<commit_message>
update dq metrics and reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="677">
   <si>
     <t xml:space="preserve">PatientIdentifikator</t>
   </si>
@@ -1996,12 +1996,6 @@
   </si>
   <si>
     <t xml:space="preserve">tracerCase_rel_py_ipat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unambiguous_rdCase_rel_py_ipat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orphaCase_rel_py_ipat</t>
   </si>
   <si>
     <t xml:space="preserve">case_no_py_ipat</t>
@@ -6474,16 +6468,10 @@
       <c r="Z1" t="s">
         <v>675</v>
       </c>
-      <c r="AA1" t="s">
-        <v>676</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>677</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B2" t="n">
         <v>2020</v>
@@ -6516,54 +6504,48 @@
         <v>190</v>
       </c>
       <c r="L2" t="n">
-        <v>750</v>
+        <v>10000</v>
       </c>
       <c r="M2" t="n">
-        <v>900</v>
+        <v>997</v>
       </c>
       <c r="N2" t="n">
-        <v>10000</v>
+        <v>950</v>
       </c>
       <c r="O2" t="n">
-        <v>997</v>
+        <v>92</v>
       </c>
       <c r="P2" t="n">
-        <v>950</v>
+        <v>100</v>
       </c>
       <c r="Q2" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R2" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="S2" t="n">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="T2" t="n">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="U2" t="n">
-        <v>19</v>
+        <v>518</v>
       </c>
       <c r="V2" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="W2" t="n">
-        <v>518</v>
+        <v>22</v>
       </c>
       <c r="X2" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Y2" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Z2" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new dq metrics for subject completeness and update resulting local reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="680">
   <si>
     <t xml:space="preserve">PatientIdentifikator</t>
   </si>
@@ -1977,6 +1977,9 @@
     <t xml:space="preserve">value_completeness_rate</t>
   </si>
   <si>
+    <t xml:space="preserve">subj_completeness_rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">case_completeness_rate</t>
   </si>
   <si>
@@ -2029,6 +2032,9 @@
   </si>
   <si>
     <t xml:space="preserve">missing_value_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incomplete_subj_no_py</t>
   </si>
   <si>
     <t xml:space="preserve">orphaMissing_no_py</t>
@@ -6474,10 +6480,16 @@
       <c r="AA1" t="s">
         <v>676</v>
       </c>
+      <c r="AB1" t="s">
+        <v>677</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B2" t="n">
         <v>2020</v>
@@ -6489,72 +6501,78 @@
         <v>96.22</v>
       </c>
       <c r="E2" t="n">
+        <v>75.05</v>
+      </c>
+      <c r="F2" t="n">
         <v>62.14</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>45</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>99.83</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>76.34</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>75</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>97.09</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>10030</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>9027</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>1906</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>997</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>950</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>92</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>100</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>90</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>19</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>3</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>518</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
+        <v>237</v>
+      </c>
+      <c r="Y2" t="n">
         <v>11</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Z2" t="n">
         <v>22</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AA2" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AB2" t="n">
         <v>25</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AC2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dq metrics and add local reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_fhirTestData_2020.xlsx
@@ -1977,7 +1977,7 @@
     <t xml:space="preserve">value_completeness_rate</t>
   </si>
   <si>
-    <t xml:space="preserve">subj_completeness_rate</t>
+    <t xml:space="preserve">subject_completeness_rate</t>
   </si>
   <si>
     <t xml:space="preserve">case_completeness_rate</t>
@@ -2034,7 +2034,7 @@
     <t xml:space="preserve">missing_value_no_py</t>
   </si>
   <si>
-    <t xml:space="preserve">incomplete_subj_no_py</t>
+    <t xml:space="preserve">incomplete_subject_no_py</t>
   </si>
   <si>
     <t xml:space="preserve">orphaMissing_no_py</t>

</xml_diff>